<commit_message>
map script, leaflet start
</commit_message>
<xml_diff>
--- a/LWC_billing.xlsx
+++ b/LWC_billing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jim Bob\Projects\LWC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B38F7A56-D81A-43BA-A6C7-73E273CE4301}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE7DEBF-1704-4179-9CE6-4977E9ADA211}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17490" windowHeight="7920" xr2:uid="{D7B7A995-59B0-4CD3-AC57-1C003558B0E8}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>Date</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>dashboard development</t>
+  </si>
+  <si>
+    <t>add plotly interaction</t>
   </si>
 </sst>
 </file>
@@ -397,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6054181-B53E-4CE9-B9EB-4021B4B1EDB9}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,6 +456,17 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43416</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>